<commit_message>
added ingredients amt && updated csv
</commit_message>
<xml_diff>
--- a/Database/ingredients.xlsx
+++ b/Database/ingredients.xlsx
@@ -1,28 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikal/Documents/School/csusm/CS441/PeasantKitchen/Database/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="13620" yWindow="620" windowWidth="15960" windowHeight="15460"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - Ingredients" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - Ingredients" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
-  <si>
-    <t>Ingredients</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>IngrID</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Butter</t>
   </si>
   <si>
@@ -117,16 +126,16 @@
   </si>
   <si>
     <t>Tomato</t>
+  </si>
+  <si>
+    <t>IngrName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -138,13 +147,13 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,14 +166,8 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="12"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -184,21 +187,6 @@
       </top>
       <bottom style="thin">
         <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -226,21 +214,6 @@
       </right>
       <top style="thin">
         <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -279,72 +252,119 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -470,7 +490,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -479,7 +499,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -488,7 +508,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -552,8 +572,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -561,7 +581,7 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
@@ -569,7 +589,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -588,7 +608,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -596,7 +616,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -624,7 +644,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -650,7 +670,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -676,7 +696,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -702,7 +722,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -728,7 +748,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -754,7 +774,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -780,7 +800,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -806,7 +826,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -832,7 +852,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -845,9 +865,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -864,7 +890,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -883,7 +909,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -909,7 +935,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -935,7 +961,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -961,7 +987,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -987,7 +1013,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1013,7 +1039,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1039,7 +1065,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1065,7 +1091,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1091,7 +1117,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1117,7 +1143,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1130,9 +1156,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1146,7 +1178,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1165,7 +1197,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1195,7 +1227,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1221,7 +1253,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1247,7 +1279,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1273,7 +1305,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1299,7 +1331,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1325,7 +1357,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1351,7 +1383,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1377,7 +1409,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1403,7 +1435,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1416,345 +1448,317 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:C34"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="1" customWidth="1"/>
-    <col min="4" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="2" width="16.33203125" style="1" customWidth="1"/>
+    <col min="3" max="255" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:2" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" t="s" s="4">
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s" s="7">
+      <c r="B4" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s" s="10">
+      <c r="B5" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s" s="10">
+      <c r="B6" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s" s="10">
+      <c r="B7" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s" s="10">
+      <c r="B8" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s" s="10">
+      <c r="B9" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s" s="10">
+      <c r="B10" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s" s="10">
+      <c r="B11" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s" s="10">
+      <c r="B12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s" s="10">
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s" s="10">
+      <c r="B14" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s" s="10">
+      <c r="B15" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s" s="10">
+      <c r="B16" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9">
-        <v>14</v>
-      </c>
-      <c r="C16" t="s" s="10">
+      <c r="B17" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s" s="10">
+      <c r="B18" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s" s="10">
+      <c r="B19" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" ht="32.35" customHeight="1">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s" s="10">
+      <c r="B20" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="5">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s" s="10">
+      <c r="B21" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" s="8"/>
-      <c r="B21" s="9">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s" s="10">
+      <c r="B22" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="5">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="8"/>
-      <c r="B22" s="9">
-        <v>20</v>
-      </c>
-      <c r="C22" t="s" s="10">
+      <c r="B23" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="5">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" ht="20.35" customHeight="1">
-      <c r="A23" s="8"/>
-      <c r="B23" s="9">
-        <v>21</v>
-      </c>
-      <c r="C23" t="s" s="10">
+      <c r="B24" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="5">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" ht="20.35" customHeight="1">
-      <c r="A24" s="8"/>
-      <c r="B24" s="9">
-        <v>22</v>
-      </c>
-      <c r="C24" t="s" s="10">
+      <c r="B25" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="5">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" ht="20.35" customHeight="1">
-      <c r="A25" s="8"/>
-      <c r="B25" s="9">
-        <v>23</v>
-      </c>
-      <c r="C25" t="s" s="10">
+      <c r="B26" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="5">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" ht="20.35" customHeight="1">
-      <c r="A26" s="8"/>
-      <c r="B26" s="9">
-        <v>24</v>
-      </c>
-      <c r="C26" t="s" s="10">
+      <c r="B27" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="5">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" ht="20.35" customHeight="1">
-      <c r="A27" s="8"/>
-      <c r="B27" s="9">
-        <v>25</v>
-      </c>
-      <c r="C27" t="s" s="10">
+      <c r="B28" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="5">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" ht="20.35" customHeight="1">
-      <c r="A28" s="8"/>
-      <c r="B28" s="9">
-        <v>26</v>
-      </c>
-      <c r="C28" t="s" s="10">
+      <c r="B29" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="5">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" ht="20.35" customHeight="1">
-      <c r="A29" s="8"/>
-      <c r="B29" s="9">
-        <v>27</v>
-      </c>
-      <c r="C29" t="s" s="10">
+      <c r="B30" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="5">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" ht="20.35" customHeight="1">
-      <c r="A30" s="8"/>
-      <c r="B30" s="9">
-        <v>28</v>
-      </c>
-      <c r="C30" t="s" s="10">
+      <c r="B31" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="5">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" ht="20.35" customHeight="1">
-      <c r="A31" s="8"/>
-      <c r="B31" s="9">
-        <v>29</v>
-      </c>
-      <c r="C31" t="s" s="10">
+      <c r="B32" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="5">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" ht="20.35" customHeight="1">
-      <c r="A32" s="8"/>
-      <c r="B32" s="9">
-        <v>30</v>
-      </c>
-      <c r="C32" t="s" s="10">
+      <c r="B33" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="5">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" ht="20.35" customHeight="1">
-      <c r="A33" s="8"/>
-      <c r="B33" s="9">
-        <v>31</v>
-      </c>
-      <c r="C33" t="s" s="10">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" ht="20.35" customHeight="1">
-      <c r="A34" s="8"/>
-      <c r="B34" s="9">
+      <c r="B34" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="C34" t="s" s="10">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>